<commit_message>
Added data model generation script
</commit_message>
<xml_diff>
--- a/mapping_files/fbref_links.xlsx
+++ b/mapping_files/fbref_links.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/simon_nyberg_accenture_com/Documents/Just for fun/fantasy-pl/mapping_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{15F3E952-164B-3548-ACCD-F47BEEE33084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7EF8C10-C277-4142-AC13-83DE47D2DD50}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{15F3E952-164B-3548-ACCD-F47BEEE33084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C59EE377-E78F-664F-91E2-B03899126718}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16680" windowHeight="20500" activeTab="1" xr2:uid="{122369B1-2B71-AB44-BF76-FF22582B9388}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="21000" activeTab="1" xr2:uid="{122369B1-2B71-AB44-BF76-FF22582B9388}"/>
   </bookViews>
   <sheets>
     <sheet name="fixtures" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="46">
   <si>
     <t>Match_Date</t>
   </si>
@@ -153,6 +153,27 @@
   </si>
   <si>
     <t>Team_Away_ID</t>
+  </si>
+  <si>
+    <t>Tottenham</t>
+  </si>
+  <si>
+    <t>Leeds United</t>
+  </si>
+  <si>
+    <t>Newcastle Utd</t>
+  </si>
+  <si>
+    <t>Nott'ham Forest</t>
+  </si>
+  <si>
+    <t>Leicester City</t>
+  </si>
+  <si>
+    <t>Manchester Utd</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
   </si>
 </sst>
 </file>
@@ -628,9 +649,9 @@
       <c r="E5">
         <v>82702941</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C5,team_codes!A:A,0))</f>
-        <v>11</v>
+        <v>#N/A</v>
       </c>
       <c r="G5">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D5,team_codes!A:A,0))</f>
@@ -653,13 +674,13 @@
       <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C6,team_codes!A:A,0))</f>
-        <v>15</v>
-      </c>
-      <c r="G6">
+        <v>#N/A</v>
+      </c>
+      <c r="G6" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D6,team_codes!A:A,0))</f>
-        <v>16</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -678,9 +699,9 @@
       <c r="E7" t="s">
         <v>27</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C7,team_codes!A:A,0))</f>
-        <v>18</v>
+        <v>#N/A</v>
       </c>
       <c r="G7">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D7,team_codes!A:A,0))</f>
@@ -728,9 +749,9 @@
       <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C9,team_codes!A:A,0))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
       <c r="G9">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D9,team_codes!A:A,0))</f>
@@ -753,9 +774,9 @@
       <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C10,team_codes!A:A,0))</f>
-        <v>14</v>
+        <v>#N/A</v>
       </c>
       <c r="G10">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D10,team_codes!A:A,0))</f>
@@ -782,9 +803,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C11,team_codes!A:A,0))</f>
         <v>19</v>
       </c>
-      <c r="G11">
+      <c r="G11" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D11,team_codes!A:A,0))</f>
-        <v>13</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -826,9 +847,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C13,team_codes!A:A,0))</f>
         <v>1</v>
       </c>
-      <c r="G13">
+      <c r="G13" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D13,team_codes!A:A,0))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -848,9 +869,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C14,team_codes!A:A,0))</f>
         <v>5</v>
       </c>
-      <c r="G14">
+      <c r="G14" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D14,team_codes!A:A,0))</f>
-        <v>15</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -866,9 +887,9 @@
       <c r="D15" t="s">
         <v>9</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C15,team_codes!A:A,0))</f>
-        <v>13</v>
+        <v>#N/A</v>
       </c>
       <c r="G15">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D15,team_codes!A:A,0))</f>
@@ -892,9 +913,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C16,team_codes!A:A,0))</f>
         <v>17</v>
       </c>
-      <c r="G16">
+      <c r="G16" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D16,team_codes!A:A,0))</f>
-        <v>11</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -936,9 +957,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C18,team_codes!A:A,0))</f>
         <v>4</v>
       </c>
-      <c r="G18">
+      <c r="G18" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D18,team_codes!A:A,0))</f>
-        <v>14</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -954,9 +975,9 @@
       <c r="D19" t="s">
         <v>23</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C19,team_codes!A:A,0))</f>
-        <v>16</v>
+        <v>#N/A</v>
       </c>
       <c r="G19">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D19,team_codes!A:A,0))</f>
@@ -980,9 +1001,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C20,team_codes!A:A,0))</f>
         <v>6</v>
       </c>
-      <c r="G20">
+      <c r="G20" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D20,team_codes!A:A,0))</f>
-        <v>18</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1020,9 +1041,9 @@
       <c r="D22" t="s">
         <v>12</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C22,team_codes!A:A,0))</f>
-        <v>18</v>
+        <v>#N/A</v>
       </c>
       <c r="G22">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D22,team_codes!A:A,0))</f>
@@ -1068,9 +1089,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C24,team_codes!A:A,0))</f>
         <v>8</v>
       </c>
-      <c r="G24">
+      <c r="G24" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D24,team_codes!A:A,0))</f>
-        <v>16</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1108,9 +1129,9 @@
       <c r="D26" t="s">
         <v>16</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C26,team_codes!A:A,0))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
       <c r="G26">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D26,team_codes!A:A,0))</f>
@@ -1152,9 +1173,9 @@
       <c r="D28" t="s">
         <v>18</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C28,team_codes!A:A,0))</f>
-        <v>11</v>
+        <v>#N/A</v>
       </c>
       <c r="G28">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D28,team_codes!A:A,0))</f>
@@ -1196,13 +1217,13 @@
       <c r="D30" t="s">
         <v>24</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C30,team_codes!A:A,0))</f>
-        <v>15</v>
-      </c>
-      <c r="G30">
+        <v>#N/A</v>
+      </c>
+      <c r="G30" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D30,team_codes!A:A,0))</f>
-        <v>13</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1218,9 +1239,9 @@
       <c r="D31" t="s">
         <v>8</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C31,team_codes!A:A,0))</f>
-        <v>14</v>
+        <v>#N/A</v>
       </c>
       <c r="G31">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D31,team_codes!A:A,0))</f>
@@ -1244,9 +1265,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C32,team_codes!A:A,0))</f>
         <v>17</v>
       </c>
-      <c r="G32">
+      <c r="G32" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D32,team_codes!A:A,0))</f>
-        <v>14</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1288,9 +1309,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C34,team_codes!A:A,0))</f>
         <v>5</v>
       </c>
-      <c r="G34">
+      <c r="G34" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D34,team_codes!A:A,0))</f>
-        <v>11</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1310,9 +1331,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C35,team_codes!A:A,0))</f>
         <v>6</v>
       </c>
-      <c r="G35">
+      <c r="G35" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D35,team_codes!A:A,0))</f>
-        <v>10</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1350,9 +1371,9 @@
       <c r="D37" t="s">
         <v>5</v>
       </c>
-      <c r="F37">
+      <c r="F37" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C37,team_codes!A:A,0))</f>
-        <v>13</v>
+        <v>#N/A</v>
       </c>
       <c r="G37">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D37,team_codes!A:A,0))</f>
@@ -1420,9 +1441,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C40,team_codes!A:A,0))</f>
         <v>20</v>
       </c>
-      <c r="G40">
+      <c r="G40" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D40,team_codes!A:A,0))</f>
-        <v>15</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -1438,13 +1459,13 @@
       <c r="D41" t="s">
         <v>15</v>
       </c>
-      <c r="F41">
+      <c r="F41" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C41,team_codes!A:A,0))</f>
-        <v>16</v>
-      </c>
-      <c r="G41">
+        <v>#N/A</v>
+      </c>
+      <c r="G41" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D41,team_codes!A:A,0))</f>
-        <v>18</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -1526,9 +1547,9 @@
       <c r="D45" t="s">
         <v>17</v>
       </c>
-      <c r="F45">
+      <c r="F45" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C45,team_codes!A:A,0))</f>
-        <v>11</v>
+        <v>#N/A</v>
       </c>
       <c r="G45">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D45,team_codes!A:A,0))</f>
@@ -1592,13 +1613,13 @@
       <c r="D48" t="s">
         <v>14</v>
       </c>
-      <c r="F48">
+      <c r="F48" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C48,team_codes!A:A,0))</f>
-        <v>13</v>
-      </c>
-      <c r="G48">
+        <v>#N/A</v>
+      </c>
+      <c r="G48" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D48,team_codes!A:A,0))</f>
-        <v>16</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -1618,9 +1639,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C49,team_codes!A:A,0))</f>
         <v>19</v>
       </c>
-      <c r="G49">
+      <c r="G49" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D49,team_codes!A:A,0))</f>
-        <v>18</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -1640,9 +1661,9 @@
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C50,team_codes!A:A,0))</f>
         <v>12</v>
       </c>
-      <c r="G50">
+      <c r="G50" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D50,team_codes!A:A,0))</f>
-        <v>15</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -1658,13 +1679,13 @@
       <c r="D51" t="s">
         <v>21</v>
       </c>
-      <c r="F51">
+      <c r="F51" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!C51,team_codes!A:A,0))</f>
-        <v>10</v>
-      </c>
-      <c r="G51">
+        <v>#N/A</v>
+      </c>
+      <c r="G51" t="e">
         <f>INDEX(team_codes!B:B,MATCH(fixtures!D51,team_codes!A:A,0))</f>
-        <v>14</v>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>
@@ -1677,12 +1698,12 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1797,7 +1818,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B11">
         <v>11</v>
@@ -1808,7 +1829,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1830,7 +1851,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1841,7 +1862,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1852,7 +1873,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1863,7 +1884,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1885,7 +1906,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B19">
         <v>18</v>

</xml_diff>